<commit_message>
BGT and WM voxel proccesing in a loop
</commit_message>
<xml_diff>
--- a/GM.xlsx
+++ b/GM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CH22"/>
+  <dimension ref="A1:CH23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -696,7 +696,7 @@
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>LWP754</t>
+          <t>LWP758</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
@@ -9922,6 +9922,438 @@
       <c r="CH22" t="inlineStr">
         <is>
           <t>5.611086e+00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>LWP758</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>7.647991e+00</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>1.217171e+00</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>7.237035e+00</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1.974221e+01</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>4.281611e+00</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>3.616100e+00</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>1.046911e+01</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>1.222028e+01</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>7.120622e+00</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>5.252108e+00</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>1.549001e+01</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>9.250815e+00</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>6.931388e+00</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>1.525038e+00</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>1.073994e+01</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>3.621569e+00</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>2.474082e+01</t>
+        </is>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>1.054749e+01</t>
+        </is>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>2.268940e+01</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>LWP758</t>
+        </is>
+      </c>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AD23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE23" t="inlineStr">
+        <is>
+          <t>3.245176e+00</t>
+        </is>
+      </c>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>2.087482e+00</t>
+        </is>
+      </c>
+      <c r="AG23" t="inlineStr">
+        <is>
+          <t>7.136637e+00</t>
+        </is>
+      </c>
+      <c r="AH23" t="inlineStr">
+        <is>
+          <t>2.210137e+00</t>
+        </is>
+      </c>
+      <c r="AI23" t="inlineStr">
+        <is>
+          <t>6.634073e+00</t>
+        </is>
+      </c>
+      <c r="AJ23" t="inlineStr">
+        <is>
+          <t>3.206725e+00</t>
+        </is>
+      </c>
+      <c r="AK23" t="inlineStr">
+        <is>
+          <t>3.321025e+00</t>
+        </is>
+      </c>
+      <c r="AL23" t="inlineStr">
+        <is>
+          <t>7.975593e+00</t>
+        </is>
+      </c>
+      <c r="AM23" t="inlineStr">
+        <is>
+          <t>5.856856e+00</t>
+        </is>
+      </c>
+      <c r="AN23" t="inlineStr">
+        <is>
+          <t>3.586366e+00</t>
+        </is>
+      </c>
+      <c r="AO23" t="inlineStr">
+        <is>
+          <t>3.826889e+00</t>
+        </is>
+      </c>
+      <c r="AP23" t="inlineStr">
+        <is>
+          <t>3.122414e+00</t>
+        </is>
+      </c>
+      <c r="AQ23" t="inlineStr">
+        <is>
+          <t>4.263797e+00</t>
+        </is>
+      </c>
+      <c r="AR23" t="inlineStr">
+        <is>
+          <t>5.489644e+00</t>
+        </is>
+      </c>
+      <c r="AS23" t="inlineStr">
+        <is>
+          <t>2.722585e+00</t>
+        </is>
+      </c>
+      <c r="AT23" t="inlineStr">
+        <is>
+          <t>9.076109e-01</t>
+        </is>
+      </c>
+      <c r="AU23" t="inlineStr">
+        <is>
+          <t>1.158232e+00</t>
+        </is>
+      </c>
+      <c r="AV23" t="inlineStr">
+        <is>
+          <t>6.309373e+00</t>
+        </is>
+      </c>
+      <c r="AW23" t="inlineStr">
+        <is>
+          <t>2.372040e+00</t>
+        </is>
+      </c>
+      <c r="AX23" t="inlineStr">
+        <is>
+          <t>2.264586e+00</t>
+        </is>
+      </c>
+      <c r="AY23" t="inlineStr">
+        <is>
+          <t>1.003864e+00</t>
+        </is>
+      </c>
+      <c r="AZ23" t="inlineStr">
+        <is>
+          <t>8.736255e+00</t>
+        </is>
+      </c>
+      <c r="BA23" t="inlineStr">
+        <is>
+          <t>LWP758</t>
+        </is>
+      </c>
+      <c r="BB23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BC23" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BD23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BE23" t="inlineStr">
+        <is>
+          <t>1.207545e+00</t>
+        </is>
+      </c>
+      <c r="BF23" t="inlineStr">
+        <is>
+          <t>2.433514e+01</t>
+        </is>
+      </c>
+      <c r="BG23" t="inlineStr">
+        <is>
+          <t>9.590888e+01</t>
+        </is>
+      </c>
+      <c r="BH23" t="inlineStr">
+        <is>
+          <t>0.000000e+00</t>
+        </is>
+      </c>
+      <c r="BI23" t="inlineStr">
+        <is>
+          <t>4.202680e-02</t>
+        </is>
+      </c>
+      <c r="BJ23" t="inlineStr">
+        <is>
+          <t>5.371094e+00</t>
+        </is>
+      </c>
+      <c r="BK23" t="inlineStr">
+        <is>
+          <t>7.020637e+00</t>
+        </is>
+      </c>
+      <c r="BL23" t="inlineStr">
+        <is>
+          <t>8.477733e+00</t>
+        </is>
+      </c>
+      <c r="BM23" t="inlineStr">
+        <is>
+          <t>8.477733e+00</t>
+        </is>
+      </c>
+      <c r="BN23" t="inlineStr">
+        <is>
+          <t>1.236412e-02</t>
+        </is>
+      </c>
+      <c r="BO23" t="inlineStr">
+        <is>
+          <t>1.194178e-02</t>
+        </is>
+      </c>
+      <c r="BP23" t="inlineStr">
+        <is>
+          <t>4.650955e+00</t>
+        </is>
+      </c>
+      <c r="BQ23" t="inlineStr">
+        <is>
+          <t>1.673508e+01</t>
+        </is>
+      </c>
+      <c r="BR23" t="inlineStr">
+        <is>
+          <t>6.515555e+01</t>
+        </is>
+      </c>
+      <c r="BS23" t="inlineStr">
+        <is>
+          <t>3.347589e-02</t>
+        </is>
+      </c>
+      <c r="BT23" t="inlineStr">
+        <is>
+          <t>-3.779603e+01</t>
+        </is>
+      </c>
+      <c r="BU23" t="inlineStr">
+        <is>
+          <t>-9.397741e+00</t>
+        </is>
+      </c>
+      <c r="BV23" t="inlineStr">
+        <is>
+          <t>2.972641e+01</t>
+        </is>
+      </c>
+      <c r="BW23" t="inlineStr">
+        <is>
+          <t>7.579457e+00</t>
+        </is>
+      </c>
+      <c r="BX23" t="inlineStr">
+        <is>
+          <t>5.930642e-02</t>
+        </is>
+      </c>
+      <c r="BY23" t="inlineStr">
+        <is>
+          <t>1.464844e+00</t>
+        </is>
+      </c>
+      <c r="BZ23" t="inlineStr">
+        <is>
+          <t>2.489279e+03</t>
+        </is>
+      </c>
+      <c r="CA23" t="inlineStr">
+        <is>
+          <t>1.845296e-01</t>
+        </is>
+      </c>
+      <c r="CB23" t="inlineStr">
+        <is>
+          <t>1.342773e+00</t>
+        </is>
+      </c>
+      <c r="CC23" t="inlineStr">
+        <is>
+          <t>1.872792e-02</t>
+        </is>
+      </c>
+      <c r="CD23" t="inlineStr">
+        <is>
+          <t>3.471696e-02</t>
+        </is>
+      </c>
+      <c r="CE23" t="inlineStr">
+        <is>
+          <t>-3.585251e-02</t>
+        </is>
+      </c>
+      <c r="CF23" t="inlineStr">
+        <is>
+          <t>1.632873e-03</t>
+        </is>
+      </c>
+      <c r="CG23" t="inlineStr">
+        <is>
+          <t>5.336861e+00</t>
+        </is>
+      </c>
+      <c r="CH23" t="inlineStr">
+        <is>
+          <t>4.519424e+00</t>
         </is>
       </c>
     </row>

</xml_diff>